<commit_message>
sprint 5 to 19
</commit_message>
<xml_diff>
--- a/ncis-sprint-burndowns.xlsx
+++ b/ncis-sprint-burndowns.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C84DC05-7F72-4908-B677-7E97B8701E2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDE0558-ED67-4300-880C-5C552B9E533D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="Sprints" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$C$1:$L$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$B$1:$L$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="136">
   <si>
     <t>Backlog Sprint</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>BA-SO</t>
+  </si>
+  <si>
+    <t>IN-DEV</t>
+  </si>
+  <si>
+    <t>BLOCK</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>READY</t>
   </si>
 </sst>
 </file>
@@ -3077,10 +3089,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C989A-0DB4-4957-8B7C-55617C9397A2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,7 +3124,9 @@
       <c r="A1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="C1" s="9" t="s">
         <v>45</v>
       </c>
@@ -3170,6 +3185,9 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
@@ -3238,6 +3256,9 @@
       <c r="A3" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
@@ -3305,7 +3326,9 @@
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
@@ -3373,7 +3396,9 @@
       <c r="A5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
@@ -3441,7 +3466,9 @@
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
@@ -3509,7 +3536,9 @@
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
@@ -3577,7 +3606,9 @@
       <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
@@ -3645,7 +3676,9 @@
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
@@ -3713,7 +3746,9 @@
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
@@ -3781,7 +3816,9 @@
       <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
@@ -3849,6 +3886,9 @@
       <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
@@ -3916,6 +3956,9 @@
       <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
@@ -4050,6 +4093,9 @@
       <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
@@ -4117,6 +4163,9 @@
       <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="B16" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C16" t="s">
         <v>49</v>
       </c>
@@ -4184,6 +4233,9 @@
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C17" t="s">
         <v>51</v>
       </c>
@@ -4253,6 +4305,9 @@
       <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="B18" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
@@ -4380,6 +4435,9 @@
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="B20" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>58</v>
       </c>
@@ -4446,6 +4504,9 @@
       <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="B21" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>60</v>
       </c>
@@ -4512,6 +4573,9 @@
       <c r="A22" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>61</v>
       </c>
@@ -4578,6 +4642,9 @@
       <c r="A23" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B23" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>62</v>
       </c>
@@ -4644,6 +4711,9 @@
       <c r="A24" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B24" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>63</v>
       </c>
@@ -4713,6 +4783,9 @@
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B25" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
@@ -4782,6 +4855,9 @@
       <c r="A26" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B26" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>65</v>
       </c>
@@ -4845,6 +4921,9 @@
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B27" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>66</v>
       </c>
@@ -4905,6 +4984,9 @@
       <c r="A28" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B28" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>67</v>
       </c>
@@ -5029,6 +5111,9 @@
       <c r="A30" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B30" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>69</v>
       </c>
@@ -5095,6 +5180,9 @@
       <c r="A31" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="B31" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>70</v>
       </c>
@@ -5155,6 +5243,9 @@
       <c r="A32" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B32" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>82</v>
       </c>
@@ -5224,6 +5315,9 @@
       <c r="A33" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B33" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>83</v>
       </c>
@@ -5250,9 +5344,9 @@
         <f t="shared" ref="I33" ca="1" si="42" xml:space="preserve"> H33 - G33</f>
         <v>5</v>
       </c>
-      <c r="J33" s="8" t="e">
-        <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R33)/(Sprints!$B$2:$B$20&gt;=R33),Sprints!$C$2:$C$20)</f>
-        <v>#N/A</v>
+      <c r="J33" s="8">
+        <f>LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R33)/(Sprints!$B$2:$B$20&gt;=R33),Sprints!$C$2:$C$20)</f>
+        <v>18</v>
       </c>
       <c r="K33" s="8" t="e">
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=S33)/(Sprints!$B$2:$B$20&gt;=S33),Sprints!$C$2:$C$20)</f>
@@ -5278,6 +5372,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>69</v>
       </c>
+      <c r="R33" s="5">
+        <v>43719</v>
+      </c>
       <c r="T33" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
@@ -5287,6 +5384,9 @@
       <c r="A34" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B34" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>84</v>
       </c>
@@ -5313,9 +5413,9 @@
         <f t="shared" ref="I34" ca="1" si="44" xml:space="preserve"> H34 - G34</f>
         <v>5</v>
       </c>
-      <c r="J34" s="8" t="e">
-        <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R34)/(Sprints!$B$2:$B$20&gt;=R34),Sprints!$C$2:$C$20)</f>
-        <v>#N/A</v>
+      <c r="J34" s="8">
+        <f>LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R34)/(Sprints!$B$2:$B$20&gt;=R34),Sprints!$C$2:$C$20)</f>
+        <v>18</v>
       </c>
       <c r="K34" s="8" t="e">
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=S34)/(Sprints!$B$2:$B$20&gt;=S34),Sprints!$C$2:$C$20)</f>
@@ -5341,6 +5441,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>63</v>
       </c>
+      <c r="R34" s="5">
+        <v>43719</v>
+      </c>
       <c r="T34" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
@@ -5350,12 +5453,15 @@
       <c r="A35" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B35" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E35" s="8">
         <f ca="1">VLOOKUP(Q35,SP!A$2:$C$9,3)</f>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F35" s="8">
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=N35)/(Sprints!$B$2:$B$20&gt;=N35),Sprints!$C$2:$C$20)</f>
@@ -5365,17 +5471,17 @@
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=O35)/(Sprints!$B$2:$B$20&gt;=O35),Sprints!$C$2:$C$20)</f>
         <v>17</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="8" t="e">
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=P35)/(Sprints!$B$2:$B$20&gt;=P35),Sprints!$C$2:$C$20)</f>
-        <v>17</v>
-      </c>
-      <c r="I35" s="8">
+        <v>#N/A</v>
+      </c>
+      <c r="I35" s="8" t="e">
         <f t="shared" ref="I35" ca="1" si="46" xml:space="preserve"> H35 - G35</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="8">
-        <f>LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R35)/(Sprints!$B$2:$B$20&gt;=R35),Sprints!$C$2:$C$20)</f>
-        <v>18</v>
+        <v>#N/A</v>
+      </c>
+      <c r="J35" s="8" t="e">
+        <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=R35)/(Sprints!$B$2:$B$20&gt;=R35),Sprints!$C$2:$C$20)</f>
+        <v>#N/A</v>
       </c>
       <c r="K35" s="8" t="e">
         <f ca="1">LOOKUP(2,1/(Sprints!$A$2:$A$20&lt;=S35)/(Sprints!$B$2:$B$20&gt;=S35),Sprints!$C$2:$C$20)</f>
@@ -5394,25 +5500,24 @@
       <c r="O35" s="5">
         <v>43696</v>
       </c>
-      <c r="P35" s="5">
-        <v>43705</v>
-      </c>
+      <c r="P35" s="5"/>
       <c r="Q35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="R35" s="5">
-        <v>43718</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="R35" s="5"/>
       <c r="T35" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B36" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>87</v>
       </c>
@@ -5470,6 +5575,9 @@
       <c r="A37" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B37" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>89</v>
       </c>
@@ -5536,6 +5644,9 @@
       <c r="A38" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B38" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>90</v>
       </c>
@@ -5602,6 +5713,9 @@
       <c r="A39" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B39" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>91</v>
       </c>
@@ -5668,6 +5782,9 @@
       <c r="A40" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B40" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>92</v>
       </c>
@@ -5730,9 +5847,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>94</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>95</v>
@@ -5788,6 +5908,9 @@
       <c r="A42" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B42" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>96</v>
       </c>
@@ -5854,6 +5977,9 @@
       <c r="A43" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B43" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>98</v>
       </c>
@@ -5920,6 +6046,9 @@
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>100</v>
       </c>
@@ -5979,9 +6108,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>94</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>101</v>
@@ -6037,6 +6169,9 @@
       <c r="A46" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B46" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>102</v>
       </c>
@@ -6097,6 +6232,9 @@
       <c r="A47" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B47" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C47" s="4" t="s">
         <v>105</v>
       </c>
@@ -6153,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>94</v>
       </c>
@@ -6214,6 +6352,9 @@
       <c r="A49" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B49" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>110</v>
       </c>
@@ -6270,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>94</v>
       </c>
@@ -6331,6 +6472,9 @@
       <c r="A51" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B51" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C51" s="4" t="s">
         <v>113</v>
       </c>
@@ -6391,6 +6535,9 @@
       <c r="A52" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B52" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C52" s="4" t="s">
         <v>115</v>
       </c>
@@ -6451,6 +6598,9 @@
       <c r="A53" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B53" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>117</v>
       </c>
@@ -6511,7 +6661,9 @@
       <c r="A54" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B54"/>
+      <c r="B54" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C54" t="s">
         <v>118</v>
       </c>
@@ -6572,7 +6724,9 @@
       <c r="A55" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B55"/>
+      <c r="B55" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C55" t="s">
         <v>119</v>
       </c>
@@ -6640,7 +6794,9 @@
       <c r="A56" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B56"/>
+      <c r="B56" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="C56" t="s">
         <v>121</v>
       </c>
@@ -6698,7 +6854,9 @@
       <c r="A57" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B57"/>
+      <c r="B57" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C57" t="s">
         <v>123</v>
       </c>
@@ -6759,7 +6917,9 @@
       <c r="A58" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B58"/>
+      <c r="B58" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C58" t="s">
         <v>125</v>
       </c>
@@ -6820,7 +6980,9 @@
       <c r="A59" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B59"/>
+      <c r="B59" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C59" t="s">
         <v>126</v>
       </c>
@@ -6881,7 +7043,9 @@
       <c r="A60" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B60"/>
+      <c r="B60" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="C60" t="s">
         <v>127</v>
       </c>
@@ -6936,7 +7100,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:L39" xr:uid="{AED31219-598C-422B-B10B-DB13322004E4}"/>
+  <autoFilter ref="B1:L60" xr:uid="{5858A0B2-01F7-4A3C-A534-0711714E3913}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="BA-SO"/>
+        <filter val="IN-DEV"/>
+        <filter val="IN-QA"/>
+        <filter val="OPEN"/>
+        <filter val="READY"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>